<commit_message>
Updated filter to be on all columns
</commit_message>
<xml_diff>
--- a/solid_edge_keyboard_assignments.xlsx
+++ b/solid_edge_keyboard_assignments.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ST7" sheetId="1" r:id="rId1"/>
     <sheet name="readme" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ST7'!$B$1:$E$789</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ST7'!$A$1:$E$789</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3967" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3969" uniqueCount="144">
   <si>
     <t>This program is free software: you can redistribute it and/or modify</t>
   </si>
@@ -448,6 +448,9 @@
   <si>
     <t>for each environment using the Solid Edge Customize dialog.</t>
   </si>
+  <si>
+    <t>updated filter to be on all columns</t>
+  </si>
 </sst>
 </file>
 
@@ -482,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -495,6 +498,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E789"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -14226,17 +14235,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E789"/>
+  <autoFilter ref="A1:E789"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C30"/>
+  <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14355,6 +14364,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>41996</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>